<commit_message>
Added link to LinkedIn post
</commit_message>
<xml_diff>
--- a/EV Sample.xlsx
+++ b/EV Sample.xlsx
@@ -22,6 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="Lookup_Counselling">Reference!$A$3:$B$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">EV!$A$1:$AR$20</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="144">
   <si>
     <t>Element</t>
   </si>
@@ -490,6 +491,10 @@
     <t>Cummu-
 lative</t>
   </si>
+  <si>
+    <t>This Excel workbook accompanies a post to LinkedIn…
+https://www.linkedin.com/pulse/use-earned-value-real-projects-greg-b-watson</t>
+  </si>
 </sst>
 </file>
 
@@ -498,7 +503,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,6 +522,14 @@
     <font>
       <sz val="11"/>
       <color theme="7" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -855,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1143,6 +1156,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1429,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,80 +1461,86 @@
     <col min="6" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C1" s="108" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="88" t="s">
         <v>109</v>
-      </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="90"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="84" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="85" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="88" t="s">
-        <v>111</v>
       </c>
       <c r="B3" s="89"/>
       <c r="C3" s="89" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="90"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="88"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="84" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="85" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="88" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="92"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="D5" s="92"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C7" s="58" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="C7" s="58" t="s">
+    <row r="9" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="C9" s="58" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C10" s="58" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:6" ht="78" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="86" t="s">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:6" ht="78" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="86" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="87"/>
-      <c r="C10" s="87" t="s">
+      <c r="B12" s="87"/>
+      <c r="C12" s="87" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="94"/>
-      <c r="E10" s="93" t="s">
+      <c r="D12" s="94"/>
+      <c r="E12" s="93" t="s">
         <v>139</v>
       </c>
-      <c r="F10" s="95" t="s">
+      <c r="F12" s="95" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1578,7 +1600,7 @@
       </c>
       <c r="B2" s="74">
         <f ca="1">SUM(EV!AF:AF)</f>
-        <v>195</v>
+        <v>209.9</v>
       </c>
       <c r="C2" s="76">
         <f ca="1">SUM(EV!AG:AG)</f>
@@ -1594,7 +1616,7 @@
       </c>
       <c r="F2" s="76">
         <f ca="1">SUM(EV!AJ:AJ)</f>
-        <v>-56.25</v>
+        <v>-71.150000000000006</v>
       </c>
       <c r="G2" s="76">
         <f ca="1">SUM(EV!AK:AK)</f>
@@ -1602,7 +1624,7 @@
       </c>
       <c r="H2" s="76">
         <f ca="1">C2/B2</f>
-        <v>0.71153846153846156</v>
+        <v>0.66102906145783702</v>
       </c>
       <c r="I2" s="76">
         <f ca="1">C2/D2</f>
@@ -1610,7 +1632,7 @@
       </c>
       <c r="J2" s="75">
         <f ca="1">(E2-C2)/(E2-B2)</f>
-        <v>1.0635593220338984</v>
+        <v>1.0817722100907941</v>
       </c>
       <c r="K2" s="72" t="s">
         <v>138</v>
@@ -1641,7 +1663,7 @@
       </c>
       <c r="B5" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A5,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Kathy</v>
+        <v>Fred</v>
       </c>
       <c r="C5" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AO$2,MATCH(A5,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1662,7 +1684,7 @@
       </c>
       <c r="B6" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A6,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Mona</v>
+        <v>Kathy</v>
       </c>
       <c r="C6" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AO$2,MATCH(A6,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1683,7 +1705,7 @@
       </c>
       <c r="B7" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A7,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Fred</v>
+        <v>Mona</v>
       </c>
       <c r="C7" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AO$2,MATCH(A7,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1977,7 +1999,7 @@
       </c>
       <c r="B21" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A21,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Zoe</v>
+        <v>Sue</v>
       </c>
       <c r="C21" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AO$2,MATCH(A21,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1998,7 +2020,7 @@
       </c>
       <c r="B22" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A22,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Sue</v>
+        <v>Zoe</v>
       </c>
       <c r="C22" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AO$2,MATCH(A22,EV!AR$3:OFFSET(EV!$AR$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -3752,7 +3774,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,23 +3903,23 @@
       </c>
       <c r="B2" s="36">
         <f>SUM(C2:AK2)</f>
-        <v>195</v>
+        <v>209.89999999999998</v>
       </c>
       <c r="C2" s="39">
         <f>SUM(C3:C102)</f>
-        <v>47</v>
+        <v>54.8</v>
       </c>
       <c r="D2" s="39">
         <f t="shared" ref="D2:AK2" si="0">SUM(D3:D102)</f>
-        <v>52</v>
+        <v>56.8</v>
       </c>
       <c r="E2" s="39">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>61.8</v>
       </c>
       <c r="F2" s="39">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>36.5</v>
       </c>
       <c r="G2" s="39">
         <f t="shared" si="0"/>
@@ -4030,16 +4052,16 @@
       </c>
       <c r="B3" s="55">
         <f>SUM(C3:AK3)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C3" s="46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" s="47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F3" s="47">
         <v>6</v>
@@ -4082,19 +4104,19 @@
       </c>
       <c r="B4" s="56">
         <f t="shared" ref="B4:B67" si="1">SUM(C4:AK4)</f>
-        <v>7</v>
+        <v>14.899999999999999</v>
       </c>
       <c r="C4" s="46">
-        <v>1</v>
+        <v>3.8</v>
       </c>
       <c r="D4" s="47">
-        <v>1</v>
+        <v>3.8</v>
       </c>
       <c r="E4" s="47">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F4" s="47">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="G4" s="47"/>
       <c r="H4" s="47"/>
@@ -4134,16 +4156,16 @@
       </c>
       <c r="B5" s="56">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5" s="47">
         <v>4</v>
       </c>
       <c r="E5" s="47">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5" s="47">
         <v>3</v>
@@ -12072,13 +12094,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AR102"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AN3" sqref="AN3"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12445,7 +12470,7 @@
       </c>
       <c r="AF3" s="16">
         <f ca="1">IFERROR(OFFSET(SAP!$B$1,MATCH(EV!$A3,SAP!$A:$A,0)-1,0),0)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AG3" s="17">
         <f ca="1">SUM(B3:AE3)</f>
@@ -12461,7 +12486,7 @@
       </c>
       <c r="AJ3" s="18">
         <f ca="1">AG3-AF3</f>
-        <v>-7.5</v>
+        <v>-13.5</v>
       </c>
       <c r="AK3" s="18">
         <f ca="1">AG3-AH3</f>
@@ -12469,7 +12494,7 @@
       </c>
       <c r="AL3" s="17">
         <f ca="1">IFERROR(AG3/AF3,0)</f>
-        <v>0.5</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="AM3" s="17">
         <f ca="1">IF(AF3=0,"",AG3/AH3)</f>
@@ -12477,7 +12502,7 @@
       </c>
       <c r="AN3" s="17">
         <f ca="1">IF(AF3=0,"",IFERROR((AI3-AG3)/(AI3-AF3),0))</f>
-        <v>1.1666666666666667</v>
+        <v>1.3461538461538463</v>
       </c>
       <c r="AO3" s="61" t="str">
         <f t="shared" ref="AO3:AO34" ca="1" si="0">IF(A3=0,"",IFERROR(VLOOKUP(IF(AND(AL3&lt;0.8,AM3&lt;0.8),"know",IF(AL3&lt;0.8,"cost",IF(AM3&lt;0.8,"sched",""))),Lookup_Counselling,2,FALSE),""))</f>
@@ -12485,15 +12510,15 @@
       </c>
       <c r="AP3" s="68">
         <f ca="1">AJ3+AK3</f>
-        <v>-15</v>
+        <v>-21</v>
       </c>
       <c r="AQ3" s="68">
         <f ca="1">IF(AP3=0,"",AP3+(1-COUNTIF(AP$3:AP3,AP3))/1000)</f>
-        <v>-15</v>
+        <v>-21</v>
       </c>
       <c r="AR3" s="67">
         <f ca="1">IF(AP3=0,"",COUNTIFS(AQ$3:AQ$20,"&lt;="&amp;AQ3))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
@@ -12623,7 +12648,7 @@
       </c>
       <c r="AF4" s="16">
         <f ca="1">IFERROR(OFFSET(SAP!$B$1,MATCH(EV!$A4,SAP!$A:$A,0)-1,0),0)</f>
-        <v>7</v>
+        <v>14.899999999999999</v>
       </c>
       <c r="AG4" s="17">
         <f t="shared" ref="AG4:AG67" ca="1" si="1">SUM(B4:AE4)</f>
@@ -12639,7 +12664,7 @@
       </c>
       <c r="AJ4" s="18">
         <f t="shared" ref="AJ4:AJ20" ca="1" si="2">AG4-AF4</f>
-        <v>8</v>
+        <v>0.10000000000000142</v>
       </c>
       <c r="AK4" s="18">
         <f t="shared" ref="AK4:AK20" ca="1" si="3">AG4-AH4</f>
@@ -12647,7 +12672,7 @@
       </c>
       <c r="AL4" s="17">
         <f t="shared" ref="AL4:AL67" ca="1" si="4">IFERROR(AG4/AF4,0)</f>
-        <v>2.1428571428571428</v>
+        <v>1.0067114093959733</v>
       </c>
       <c r="AM4" s="17">
         <f t="shared" ref="AM4:AM67" ca="1" si="5">IF(AF4=0,"",AG4/AH4)</f>
@@ -12655,7 +12680,7 @@
       </c>
       <c r="AN4" s="17">
         <f t="shared" ref="AN4:AN67" ca="1" si="6">IF(AF4=0,"",IFERROR((AI4-AG4)/(AI4-AF4),0))</f>
-        <v>0.84905660377358494</v>
+        <v>0.99778270509977829</v>
       </c>
       <c r="AO4" s="61" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -12663,15 +12688,15 @@
       </c>
       <c r="AP4" s="68">
         <f t="shared" ref="AP4:AP67" ca="1" si="7">AJ4+AK4</f>
-        <v>8</v>
+        <v>0.10000000000000142</v>
       </c>
       <c r="AQ4" s="68">
         <f ca="1">IF(AP4=0,"",AP4+(1-COUNTIF(AP$3:AP4,AP4))/1000)</f>
-        <v>8</v>
+        <v>0.10000000000000142</v>
       </c>
       <c r="AR4" s="67">
         <f t="shared" ref="AR4:AR67" ca="1" si="8">IF(AP4=0,"",COUNTIFS(AQ$3:AQ$20,"&lt;="&amp;AQ4))</f>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
@@ -12801,7 +12826,7 @@
       </c>
       <c r="AF5" s="16">
         <f ca="1">IFERROR(OFFSET(SAP!$B$1,MATCH(EV!$A5,SAP!$A:$A,0)-1,0),0)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AG5" s="17">
         <f t="shared" ca="1" si="1"/>
@@ -12817,7 +12842,7 @@
       </c>
       <c r="AJ5" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK5" s="18">
         <f t="shared" ca="1" si="3"/>
@@ -12825,7 +12850,7 @@
       </c>
       <c r="AL5" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.25</v>
+        <v>1.1538461538461537</v>
       </c>
       <c r="AM5" s="17">
         <f t="shared" ca="1" si="5"/>
@@ -12833,7 +12858,7 @@
       </c>
       <c r="AN5" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.9375</v>
+        <v>0.95744680851063835</v>
       </c>
       <c r="AO5" s="61" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -12841,15 +12866,15 @@
       </c>
       <c r="AP5" s="68">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AQ5" s="68">
         <f ca="1">IF(AP5=0,"",AP5+(1-COUNTIF(AP$3:AP5,AP5))/1000)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR5" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
@@ -14629,7 +14654,7 @@
       </c>
       <c r="AR15" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
@@ -14807,7 +14832,7 @@
       </c>
       <c r="AR16" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
@@ -29627,9 +29652,14 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="45" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"-,Bold"&amp;F
+&amp;A</oddHeader>
+    <oddFooter>&amp;LPrinted &amp;D &amp;T&amp;RPage &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Corrected VAC calculation in another place
</commit_message>
<xml_diff>
--- a/EV Sample.xlsx
+++ b/EV Sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg.B.Watson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg.B.Watson\Documents\GitHub\CrunchThePeople1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -496,7 +496,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> The tab "CallList" lists the rows from the EV tab in order of their priority as determined by the calculations on the EV tab.
-Recall that the formula we apply for "estimate at completion" (EAC) assumes that each student will continue to study with the same efficiency until they complete. Thus the EAC = AC + (BAC - EV) / (CPI * SPI),  the inclusion of SPI in the denominator that the schedule will extend in time until the course is complete
+Recall that the formula we apply for "estimate at completion" (EAC) assumes that each student will continue to study with the same efficiency until they complete, because even though each course has deadlines, each student is able to continue the same course in a following cycle. Thus the EAC = AC + (BAC - EV) / (CPI * SPI),  the inclusion of SPI in the denominator that the schedule will extend in time until the course is complete
 Raw Priority = VAC = BAC - EAC 
 A challenge with "raw priority" is that some rows may have the same VAC. For each row that has the same VAC, we add a small amount so that they are listed in sequence.</t>
     </r>
@@ -1454,7 +1454,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1514,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="C9" s="58" t="s">
         <v>145</v>
       </c>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1559,8 +1559,8 @@
   <dimension ref="A1:M104"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,12 +1643,12 @@
         <v>0.51388888888888884</v>
       </c>
       <c r="J2" s="75">
-        <f ca="1">B2+(E2-C2)/(H2)</f>
-        <v>1633.8162162162164</v>
+        <f ca="1">B2+(E2-C2)/(H2*I2)</f>
+        <v>2980.7639883126376</v>
       </c>
       <c r="K2" s="75">
         <f ca="1">E2-J2</f>
-        <v>-553.81621621621639</v>
+        <v>-1900.7639883126376</v>
       </c>
       <c r="L2" s="75">
         <f ca="1">(E2-C2)/(E2-B2)</f>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="B5" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A5,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Fred</v>
+        <v>Kathy</v>
       </c>
       <c r="C5" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A5,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B6" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A6,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Kathy</v>
+        <v>Mona</v>
       </c>
       <c r="C6" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A6,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="B7" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A7,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Mona</v>
+        <v>Ted</v>
       </c>
       <c r="C7" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A7,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1754,7 +1754,7 @@
       </c>
       <c r="B8" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A8,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Judy</v>
+        <v>Mike</v>
       </c>
       <c r="C8" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A8,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="B9" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A9,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Lynda</v>
+        <v>Stu</v>
       </c>
       <c r="C9" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A9,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="B10" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A10,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Ted</v>
+        <v>Fred</v>
       </c>
       <c r="C10" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A10,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1823,11 +1823,11 @@
       </c>
       <c r="B11" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A11,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Henry</v>
+        <v>Nancy</v>
       </c>
       <c r="C11" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A11,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>May be having difficulty with the material</v>
+        <v>Not completing milestones in the week due</v>
       </c>
       <c r="D11" s="77"/>
       <c r="E11" s="77"/>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="B12" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A12,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Tom</v>
+        <v>Judy</v>
       </c>
       <c r="C12" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A12,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B13" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A13,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Mike</v>
+        <v>Lynda</v>
       </c>
       <c r="C13" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A13,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="B14" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A14,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Dick</v>
+        <v>Henry</v>
       </c>
       <c r="C14" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A14,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="B15" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A15,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Stu</v>
+        <v>Tom</v>
       </c>
       <c r="C15" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A15,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1938,11 +1938,11 @@
       </c>
       <c r="B16" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A16,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Harry</v>
+        <v>Dick</v>
       </c>
       <c r="C16" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A16,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Charging time to the wrong SAP code</v>
+        <v>May be having difficulty with the material</v>
       </c>
       <c r="D16" s="77"/>
       <c r="E16" s="77"/>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B17" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A17,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Frank</v>
+        <v>Bill</v>
       </c>
       <c r="C17" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A17,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="B18" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A18,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Bill</v>
+        <v>Kurt</v>
       </c>
       <c r="C18" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A18,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="B19" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A19,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Kurt</v>
+        <v>Frank</v>
       </c>
       <c r="C19" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A19,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
@@ -2030,11 +2030,11 @@
       </c>
       <c r="B20" s="82" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$A$2,MATCH($A20,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Nancy</v>
+        <v>Harry</v>
       </c>
       <c r="C20" s="83" t="str">
         <f ca="1">IFERROR(OFFSET(EV!$AP$2,MATCH(A20,EV!AS$3:OFFSET(EV!$AS$1,MATCH(0,EV!$A:$A,0)-2,0),0),0),"")</f>
-        <v>Not completing milestones in the week due</v>
+        <v>Charging time to the wrong SAP code</v>
       </c>
       <c r="D20" s="77"/>
       <c r="E20" s="77"/>
@@ -12325,7 +12325,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AN3" sqref="AN3"/>
+      <selection pane="bottomRight" activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12727,8 +12727,8 @@
         <v>0.5</v>
       </c>
       <c r="AN3" s="17">
-        <f ca="1">IF(AF3=0,"",AF3 + (AI3 - AG3)/(AL3))</f>
-        <v>168</v>
+        <f ca="1">IF(AF3=0,"",AF3 + (AI3 - AG3)/(AL3*AM3))</f>
+        <v>315</v>
       </c>
       <c r="AO3" s="17">
         <f ca="1">IF(AF3=0,"",IFERROR((AI3-AG3)/(AI3-AF3),0))</f>
@@ -12740,15 +12740,15 @@
       </c>
       <c r="AQ3" s="68">
         <f ca="1">IF(AF3=0,0,AI3-AN3)</f>
-        <v>-108</v>
+        <v>-255</v>
       </c>
       <c r="AR3" s="68">
         <f ca="1">IF(AQ3=0,"",AQ3+(1-COUNTIF(AQ$3:AQ3,AQ3))/1000)</f>
-        <v>-108</v>
+        <v>-255</v>
       </c>
       <c r="AS3" s="67">
         <f ca="1">IF(AQ3=0,"",COUNTIFS(AR$3:AR$20,"&lt;="&amp;AR3))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
@@ -12909,7 +12909,7 @@
         <v>1</v>
       </c>
       <c r="AN4" s="17">
-        <f t="shared" ref="AN4:AN67" ca="1" si="6">IF(AF4=0,"",AF4 + (AI4 - AG4)/(AL4))</f>
+        <f t="shared" ref="AN4:AN67" ca="1" si="6">IF(AF4=0,"",AF4 + (AI4 - AG4)/(AL4*AM4))</f>
         <v>59.599999999999994</v>
       </c>
       <c r="AO4" s="17">
@@ -13274,7 +13274,7 @@
       </c>
       <c r="AN6" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="AO6" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -13286,15 +13286,15 @@
       </c>
       <c r="AQ6" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-12</v>
+        <v>-75</v>
       </c>
       <c r="AR6" s="68">
         <f ca="1">IF(AQ6=0,"",AQ6+(1-COUNTIF(AQ$3:AQ6,AQ6))/1000)</f>
-        <v>-12</v>
+        <v>-75</v>
       </c>
       <c r="AS6" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
@@ -13456,7 +13456,7 @@
       </c>
       <c r="AN7" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>96</v>
+        <v>366</v>
       </c>
       <c r="AO7" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -13468,15 +13468,15 @@
       </c>
       <c r="AQ7" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-36</v>
+        <v>-306</v>
       </c>
       <c r="AR7" s="68">
         <f ca="1">IF(AQ7=0,"",AQ7+(1-COUNTIF(AQ$3:AQ7,AQ7))/1000)</f>
-        <v>-36</v>
+        <v>-306</v>
       </c>
       <c r="AS7" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
@@ -13638,7 +13638,7 @@
       </c>
       <c r="AN8" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>74.666666666666657</v>
+        <v>94.8888888888889</v>
       </c>
       <c r="AO8" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -13650,15 +13650,15 @@
       </c>
       <c r="AQ8" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.666666666666657</v>
+        <v>-34.8888888888889</v>
       </c>
       <c r="AR8" s="68">
         <f ca="1">IF(AQ8=0,"",AQ8+(1-COUNTIF(AQ$3:AQ8,AQ8))/1000)</f>
-        <v>-14.666666666666657</v>
+        <v>-34.8888888888889</v>
       </c>
       <c r="AS8" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
@@ -13820,7 +13820,7 @@
       </c>
       <c r="AN9" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>64</v>
+        <v>244</v>
       </c>
       <c r="AO9" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -13832,15 +13832,15 @@
       </c>
       <c r="AQ9" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-4</v>
+        <v>-184</v>
       </c>
       <c r="AR9" s="68">
         <f ca="1">IF(AQ9=0,"",AQ9+(1-COUNTIF(AQ$3:AQ9,AQ9))/1000)</f>
-        <v>-4</v>
+        <v>-184</v>
       </c>
       <c r="AS9" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
@@ -14002,7 +14002,7 @@
       </c>
       <c r="AN10" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="AO10" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -14014,15 +14014,15 @@
       </c>
       <c r="AQ10" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-12</v>
+        <v>-75</v>
       </c>
       <c r="AR10" s="68">
         <f ca="1">IF(AQ10=0,"",AQ10+(1-COUNTIF(AQ$3:AQ10,AQ10))/1000)</f>
-        <v>-12.000999999999999</v>
+        <v>-75.001000000000005</v>
       </c>
       <c r="AS10" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
@@ -14184,7 +14184,7 @@
       </c>
       <c r="AN11" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>112</v>
+        <v>427</v>
       </c>
       <c r="AO11" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -14196,15 +14196,15 @@
       </c>
       <c r="AQ11" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-52</v>
+        <v>-367</v>
       </c>
       <c r="AR11" s="68">
         <f ca="1">IF(AQ11=0,"",AQ11+(1-COUNTIF(AQ$3:AQ11,AQ11))/1000)</f>
-        <v>-52</v>
+        <v>-367</v>
       </c>
       <c r="AS11" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
@@ -14366,7 +14366,7 @@
       </c>
       <c r="AN12" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>104.00000000000001</v>
+        <v>195.00000000000003</v>
       </c>
       <c r="AO12" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -14378,15 +14378,15 @@
       </c>
       <c r="AQ12" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-44.000000000000014</v>
+        <v>-135.00000000000003</v>
       </c>
       <c r="AR12" s="68">
         <f ca="1">IF(AQ12=0,"",AQ12+(1-COUNTIF(AQ$3:AQ12,AQ12))/1000)</f>
-        <v>-44.000000000000014</v>
+        <v>-135.00000000000003</v>
       </c>
       <c r="AS12" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
@@ -14548,7 +14548,7 @@
       </c>
       <c r="AN13" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>96</v>
+        <v>180</v>
       </c>
       <c r="AO13" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -14560,15 +14560,15 @@
       </c>
       <c r="AQ13" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-36</v>
+        <v>-120</v>
       </c>
       <c r="AR13" s="68">
         <f ca="1">IF(AQ13=0,"",AQ13+(1-COUNTIF(AQ$3:AQ13,AQ13))/1000)</f>
-        <v>-36.000999999999998</v>
+        <v>-120</v>
       </c>
       <c r="AS13" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -14750,7 +14750,7 @@
       </c>
       <c r="AS14" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
@@ -14912,7 +14912,7 @@
       </c>
       <c r="AN15" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>128</v>
+        <v>488</v>
       </c>
       <c r="AO15" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -14924,15 +14924,15 @@
       </c>
       <c r="AQ15" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-68</v>
+        <v>-428</v>
       </c>
       <c r="AR15" s="68">
         <f ca="1">IF(AQ15=0,"",AQ15+(1-COUNTIF(AQ$3:AQ15,AQ15))/1000)</f>
-        <v>-68</v>
+        <v>-428</v>
       </c>
       <c r="AS15" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
@@ -15094,7 +15094,7 @@
       </c>
       <c r="AN16" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>160</v>
+        <v>610</v>
       </c>
       <c r="AO16" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -15106,15 +15106,15 @@
       </c>
       <c r="AQ16" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-100</v>
+        <v>-550</v>
       </c>
       <c r="AR16" s="68">
         <f ca="1">IF(AQ16=0,"",AQ16+(1-COUNTIF(AQ$3:AQ16,AQ16))/1000)</f>
-        <v>-100</v>
+        <v>-550</v>
       </c>
       <c r="AS16" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.25">
@@ -15276,7 +15276,7 @@
       </c>
       <c r="AN17" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="AO17" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -15288,15 +15288,15 @@
       </c>
       <c r="AQ17" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-52</v>
+        <v>-150</v>
       </c>
       <c r="AR17" s="68">
         <f ca="1">IF(AQ17=0,"",AQ17+(1-COUNTIF(AQ$3:AQ17,AQ17))/1000)</f>
-        <v>-52.000999999999998</v>
+        <v>-150</v>
       </c>
       <c r="AS17" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.25">
@@ -15458,7 +15458,7 @@
       </c>
       <c r="AN18" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="AO18" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -15470,15 +15470,15 @@
       </c>
       <c r="AQ18" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-52</v>
+        <v>-150</v>
       </c>
       <c r="AR18" s="68">
         <f ca="1">IF(AQ18=0,"",AQ18+(1-COUNTIF(AQ$3:AQ18,AQ18))/1000)</f>
-        <v>-52.002000000000002</v>
+        <v>-150.001</v>
       </c>
       <c r="AS18" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.25">
@@ -15640,7 +15640,7 @@
       </c>
       <c r="AN19" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>104.00000000000001</v>
+        <v>195.00000000000003</v>
       </c>
       <c r="AO19" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -15652,15 +15652,15 @@
       </c>
       <c r="AQ19" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-44.000000000000014</v>
+        <v>-135.00000000000003</v>
       </c>
       <c r="AR19" s="68">
         <f ca="1">IF(AQ19=0,"",AQ19+(1-COUNTIF(AQ$3:AQ19,AQ19))/1000)</f>
-        <v>-44.001000000000012</v>
+        <v>-135.00100000000003</v>
       </c>
       <c r="AS19" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.25">
@@ -15822,7 +15822,7 @@
       </c>
       <c r="AN20" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>96</v>
+        <v>366</v>
       </c>
       <c r="AO20" s="17">
         <f t="shared" ca="1" si="7"/>
@@ -15834,15 +15834,15 @@
       </c>
       <c r="AQ20" s="68">
         <f t="shared" ca="1" si="8"/>
-        <v>-36</v>
+        <v>-306</v>
       </c>
       <c r="AR20" s="68">
         <f ca="1">IF(AQ20=0,"",AQ20+(1-COUNTIF(AQ$3:AQ20,AQ20))/1000)</f>
-        <v>-36.002000000000002</v>
+        <v>-306.00099999999998</v>
       </c>
       <c r="AS20" s="67">
         <f t="shared" ca="1" si="9"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.25">
@@ -24269,7 +24269,7 @@
         <v/>
       </c>
       <c r="AN68" s="17" t="str">
-        <f t="shared" ref="AN68:AN102" ca="1" si="15">IF(AF68=0,"",AF68 + (AI68 - AG68)/(AL68))</f>
+        <f t="shared" ref="AN68:AN102" ca="1" si="15">IF(AF68=0,"",AF68 + (AI68 - AG68)/(AL68*AM68))</f>
         <v/>
       </c>
       <c r="AO68" s="17" t="str">

</xml_diff>